<commit_message>
Adicionado a estrutura básica do projeto, components, models, services, e enums.
</commit_message>
<xml_diff>
--- a/Backend-Spring-Boot/src/main/resources/upload.xlsx
+++ b/Backend-Spring-Boot/src/main/resources/upload.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>RELATÓRIO MONITORADORES</t>
   </si>
@@ -98,39 +98,24 @@
     <t>Jurídica</t>
   </si>
   <si>
-    <t>11223344556677</t>
-  </si>
-  <si>
-    <t>Companhia de Tecnologia</t>
-  </si>
-  <si>
-    <t>3133334444</t>
-  </si>
-  <si>
-    <t>contato@tecnologia.com</t>
-  </si>
-  <si>
-    <t>IE1234568</t>
+    <t>55667788990011</t>
+  </si>
+  <si>
+    <t>Construtora Nova Era Ltda</t>
+  </si>
+  <si>
+    <t>1133445566</t>
+  </si>
+  <si>
+    <t>contato@construtorane.com</t>
+  </si>
+  <si>
+    <t>IE334455</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>55667788990011</t>
-  </si>
-  <si>
-    <t>Construtora Nova Era Ltda</t>
-  </si>
-  <si>
-    <t>1133445566</t>
-  </si>
-  <si>
-    <t>contato@construtorane.com</t>
-  </si>
-  <si>
-    <t>IE334455</t>
-  </si>
-  <si>
     <t>99887766554433</t>
   </si>
   <si>
@@ -234,6 +219,36 @@
   </si>
   <si>
     <t>55666777</t>
+  </si>
+  <si>
+    <t>04596017174</t>
+  </si>
+  <si>
+    <t>Rafael Gibson</t>
+  </si>
+  <si>
+    <t>62998892724</t>
+  </si>
+  <si>
+    <t>exemplo@email.com</t>
+  </si>
+  <si>
+    <t>4986532</t>
+  </si>
+  <si>
+    <t>14586952478</t>
+  </si>
+  <si>
+    <t>Rafael Cadastro</t>
+  </si>
+  <si>
+    <t>62998889568</t>
+  </si>
+  <si>
+    <t>exemplo@gmail.com</t>
+  </si>
+  <si>
+    <t>145582</t>
   </si>
 </sst>
 </file>
@@ -358,12 +373,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -379,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -519,7 +536,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="2">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="B6" t="s" s="2">
         <v>27</v>
@@ -548,7 +565,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n" s="2">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="B7" t="s" s="2">
         <v>27</v>
@@ -572,41 +589,41 @@
         <v>33</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="2">
-        <v>26.0</v>
+        <v>2.0</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="H8" t="n" s="2">
+        <v>32872.0</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="2">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
       <c r="B9" t="s" s="2">
         <v>10</v>
@@ -627,7 +644,7 @@
         <v>49</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>32872.0</v>
+        <v>31239.0</v>
       </c>
       <c r="I9" t="s" s="2">
         <v>16</v>
@@ -635,7 +652,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n" s="2">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="B10" t="s" s="2">
         <v>10</v>
@@ -644,19 +661,19 @@
         <v>50</v>
       </c>
       <c r="D10" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="E10" t="s" s="2">
+      <c r="F10" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="F10" t="s" s="2">
+      <c r="G10" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="G10" t="s" s="2">
-        <v>54</v>
-      </c>
       <c r="H10" t="n" s="2">
-        <v>31239.0</v>
+        <v>33690.0</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>16</v>
@@ -664,16 +681,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n" s="2">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="B11" t="s" s="2">
         <v>10</v>
       </c>
       <c r="C11" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>18</v>
       </c>
       <c r="E11" t="s" s="2">
         <v>56</v>
@@ -685,15 +702,15 @@
         <v>58</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>33690.0</v>
+        <v>28794.0</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="2">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="B12" t="s" s="2">
         <v>10</v>
@@ -714,15 +731,15 @@
         <v>63</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>28794.0</v>
+        <v>33007.0</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="2">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="B13" t="s" s="2">
         <v>10</v>
@@ -743,7 +760,7 @@
         <v>68</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>33007.0</v>
+        <v>30581.0</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>16</v>
@@ -751,7 +768,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n" s="2">
-        <v>34.0</v>
+        <v>43.0</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>10</v>
@@ -772,9 +789,38 @@
         <v>73</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>30581.0</v>
+        <v>45307.0</v>
       </c>
       <c r="I14" t="s" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="2">
+        <v>44.0</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="H15" t="n" s="2">
+        <v>45308.0</v>
+      </c>
+      <c r="I15" t="s" s="2">
         <v>16</v>
       </c>
     </row>

</xml_diff>